<commit_message>
bug fixed for canopy cover bug fixed for replantig
still bugs in multilayer mode when replanting
some unexpected bug running 2B for soroe
</commit_message>
<xml_diff>
--- a/software/3D-CMCC-Forest-Model/tables/rain_interception.xlsx
+++ b/software/3D-CMCC-Forest-Model/tables/rain_interception.xlsx
@@ -24,16 +24,16 @@
     <t>LAI</t>
   </si>
   <si>
-    <t>INT (jiao et al., 2016)</t>
-  </si>
-  <si>
-    <t>%  (jiao et al., 2016)</t>
-  </si>
-  <si>
     <t>INT (Lawrence et al., 2006)</t>
   </si>
   <si>
     <t>%  (Lawrence et al., 2006)</t>
+  </si>
+  <si>
+    <t>INT (Jiao et al., 2016)</t>
+  </si>
+  <si>
+    <t>%  (Jiao et al., 2016)</t>
   </si>
 </sst>
 </file>
@@ -100,7 +100,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>%  (jiao et al., 2016)</c:v>
+                  <c:v>%  (Jiao et al., 2016)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -813,7 +813,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -834,16 +834,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>